<commit_message>
finish ID DEQ themes
</commit_message>
<xml_diff>
--- a/Vocabularies/ID/id-deq-g.xlsx
+++ b/Vocabularies/ID/id-deq-g.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph/Library/Containers/com.microsoft.Excel/Data/Desktop/WSWC/IoW/Vocabularies/ID/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kso8/Box/Internet Of Water/GitHub/Glossary/Vocabularies/ID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31909EEA-9542-8547-8096-00FCBED8CD99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A70E46-4FA7-2A40-BEC1-62D2D399B938}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
+    <workbookView xWindow="-38400" yWindow="1180" windowWidth="38400" windowHeight="21140" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="883">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -3045,8 +3045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E542F74-ACD9-49CD-B312-AB6D05B8D550}">
   <dimension ref="A1:I418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E304" sqref="E304"/>
+    <sheetView tabSelected="1" topLeftCell="A383" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D419" sqref="D419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3289,7 +3289,9 @@
       <c r="C17" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -3581,7 +3583,9 @@
       <c r="C41" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -3660,7 +3664,9 @@
       <c r="C47" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
@@ -3898,7 +3904,9 @@
       <c r="C65" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="D65" s="3"/>
+      <c r="D65" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
@@ -3921,7 +3929,9 @@
       <c r="C67" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="D67" s="3"/>
+      <c r="D67" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
@@ -4031,7 +4041,9 @@
       <c r="C75" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="D75" s="3"/>
+      <c r="D75" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -4082,7 +4094,9 @@
       <c r="C79" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="D79" s="3"/>
+      <c r="D79" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
@@ -4108,7 +4122,12 @@
       <c r="C81" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="D81" s="3"/>
+      <c r="D81" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E81" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
@@ -4251,7 +4270,9 @@
       <c r="C92" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="D92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
@@ -4508,7 +4529,9 @@
       <c r="C112" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="D112" s="3"/>
+      <c r="D112" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
@@ -4517,7 +4540,9 @@
       <c r="C113" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="D113" s="3"/>
+      <c r="D113" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
@@ -4590,7 +4615,9 @@
       <c r="C119" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="D119" s="3"/>
+      <c r="D119" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
@@ -4727,7 +4754,9 @@
       <c r="C130" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="D130" s="3"/>
+      <c r="D130" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
@@ -4736,7 +4765,9 @@
       <c r="C131" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="D131" s="3"/>
+      <c r="D131" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
@@ -4745,7 +4776,9 @@
       <c r="C132" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="D132" s="3"/>
+      <c r="D132" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
@@ -4829,7 +4862,9 @@
       <c r="C139" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="D139" s="3"/>
+      <c r="D139" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
@@ -5022,7 +5057,9 @@
       <c r="C154" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="D154" s="3"/>
+      <c r="D154" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
@@ -5131,7 +5168,9 @@
       <c r="C163" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="D163" s="3"/>
+      <c r="D163" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
@@ -5143,6 +5182,12 @@
       <c r="D164" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="E164" t="s">
+        <v>9</v>
+      </c>
+      <c r="F164" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
@@ -5287,7 +5332,9 @@
       <c r="C176" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="D176" s="3"/>
+      <c r="D176" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
@@ -5463,7 +5510,12 @@
       <c r="C190" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="D190" s="3"/>
+      <c r="D190" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E190" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
@@ -5472,7 +5524,9 @@
       <c r="C191" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="D191" s="3"/>
+      <c r="D191" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
@@ -5564,7 +5618,9 @@
       <c r="C199" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="D199" s="3"/>
+      <c r="D199" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
@@ -6113,7 +6169,9 @@
       <c r="C245" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="D245" s="3"/>
+      <c r="D245" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
@@ -6236,7 +6294,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>270</v>
       </c>
@@ -6247,7 +6305,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>271</v>
       </c>
@@ -6258,7 +6316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>272</v>
       </c>
@@ -6269,7 +6327,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>273</v>
       </c>
@@ -6283,7 +6341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>274</v>
       </c>
@@ -6297,7 +6355,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>275</v>
       </c>
@@ -6308,7 +6366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>276</v>
       </c>
@@ -6319,7 +6377,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>277</v>
       </c>
@@ -6330,7 +6388,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>278</v>
       </c>
@@ -6344,7 +6402,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>279</v>
       </c>
@@ -6355,7 +6413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>280</v>
       </c>
@@ -6366,7 +6424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>281</v>
       </c>
@@ -6377,7 +6435,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>282</v>
       </c>
@@ -6388,7 +6446,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>283</v>
       </c>
@@ -6401,8 +6459,11 @@
       <c r="E270" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F270" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>284</v>
       </c>
@@ -6415,8 +6476,11 @@
       <c r="E271" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F271" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>285</v>
       </c>
@@ -6428,6 +6492,12 @@
       </c>
       <c r="E272" t="s">
         <v>19</v>
+      </c>
+      <c r="F272" t="s">
+        <v>10</v>
+      </c>
+      <c r="G272" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.2">
@@ -6440,6 +6510,9 @@
       <c r="D273" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E273" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
@@ -6658,7 +6731,9 @@
       <c r="C292" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="D292" s="3"/>
+      <c r="D292" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
@@ -6778,7 +6853,9 @@
       <c r="C302" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="D302" s="3"/>
+      <c r="D302" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
@@ -6805,7 +6882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
         <v>318</v>
       </c>
@@ -6819,15 +6896,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>319</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D306" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
         <v>320</v>
       </c>
@@ -6841,892 +6921,1390 @@
         <v>24</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>321</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D308" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
         <v>322</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D309" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>323</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D310" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
         <v>324</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D311" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
         <v>325</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D312" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
         <v>326</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D313" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E313" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
         <v>327</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D314" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" s="1" t="s">
         <v>328</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D315" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
         <v>329</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D316" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E316" t="s">
+        <v>23</v>
+      </c>
+      <c r="F316" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
         <v>330</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D317" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E317" t="s">
+        <v>14</v>
+      </c>
+      <c r="F317" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
         <v>331</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D318" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E318" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
         <v>332</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D319" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
         <v>333</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D320" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E320" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
         <v>334</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D321" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>335</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D322" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E322" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" s="1" t="s">
         <v>336</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D323" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E323" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>337</v>
       </c>
       <c r="C324" s="2" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D324" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E324" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>338</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D325" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>339</v>
       </c>
       <c r="C326" s="2" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D326" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
         <v>340</v>
       </c>
       <c r="C327" s="2" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D327" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
         <v>341</v>
       </c>
       <c r="C328" s="2" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D328" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" s="1" t="s">
         <v>342</v>
       </c>
       <c r="C329" s="2" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D329" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
         <v>343</v>
       </c>
       <c r="C330" s="2" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D330" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A331" s="1" t="s">
         <v>344</v>
       </c>
       <c r="C331" s="2" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D331" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E331" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
         <v>345</v>
       </c>
       <c r="C332" s="2" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D332" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
         <v>346</v>
       </c>
       <c r="C333" s="2" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D333" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>347</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D334" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A335" s="1" t="s">
         <v>348</v>
       </c>
       <c r="C335" s="2" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D335" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
         <v>349</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D336" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A337" s="1" t="s">
         <v>350</v>
       </c>
       <c r="C337" s="2" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D337" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>351</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D338" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A339" s="1" t="s">
         <v>352</v>
       </c>
       <c r="C339" s="2" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D339" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>353</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D340" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A341" s="1" t="s">
         <v>354</v>
       </c>
       <c r="C341" s="2" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D341" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
         <v>355</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D342" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E342" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F342" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
         <v>356</v>
       </c>
       <c r="C343" s="2" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D343" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E343" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
         <v>357</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D344" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A345" s="1" t="s">
         <v>358</v>
       </c>
       <c r="C345" s="2" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D345" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A346" s="1" t="s">
         <v>359</v>
       </c>
       <c r="C346" s="2" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D346" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E346" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
         <v>360</v>
       </c>
       <c r="C347" s="2" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D347" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E347" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
         <v>361</v>
       </c>
       <c r="C348" s="2" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D348" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E348" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C349" s="2" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D349" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E349" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>363</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D350" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
         <v>364</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D351" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D352" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A353" s="1" t="s">
         <v>366</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D353" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E353" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D354" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
         <v>368</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D355" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>369</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D356" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
         <v>370</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D357" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
         <v>371</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D358" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
         <v>372</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D359" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E359" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
         <v>373</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D360" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="s">
         <v>374</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D361" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E361" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
         <v>375</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D362" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E362" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A363" s="1" t="s">
         <v>376</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D363" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E363" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
         <v>377</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D364" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E364" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A365" s="1" t="s">
         <v>378</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D365" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E365" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>379</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D366" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E366" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A367" s="1" t="s">
         <v>380</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D367" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E367" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
         <v>381</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D368" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A369" s="1" t="s">
         <v>382</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D369" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
         <v>383</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D370" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E370" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A371" s="1" t="s">
         <v>384</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>798</v>
       </c>
-    </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D371" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E371" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A372" s="1" t="s">
         <v>385</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D372" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A373" s="1" t="s">
         <v>386</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D373" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
         <v>387</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D374" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A375" s="1" t="s">
         <v>388</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D375" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E375" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
         <v>389</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D376" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E376" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A377" s="1" t="s">
         <v>390</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D377" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
         <v>391</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D378" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D379" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A380" s="1" t="s">
         <v>393</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D380" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A381" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D381" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A382" s="1" t="s">
         <v>395</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D382" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E382" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F382" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A383" s="1" t="s">
         <v>396</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D383" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A384" s="1" t="s">
         <v>397</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D384" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A385" s="1" t="s">
         <v>398</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D385" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A386" s="1" t="s">
         <v>399</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D386" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A387" s="1" t="s">
         <v>400</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D387" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A388" s="1" t="s">
         <v>401</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D388" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A389" s="1" t="s">
         <v>402</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D389" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A390" s="1" t="s">
         <v>403</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D390" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E390" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A391" s="1" t="s">
         <v>404</v>
       </c>
       <c r="C391" s="2" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D391" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E391" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A392" s="1" t="s">
         <v>405</v>
       </c>
       <c r="C392" s="2" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D392" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E392" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A393" s="1" t="s">
         <v>406</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D393" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E393" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
         <v>407</v>
       </c>
       <c r="C394" s="2" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D394" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E394" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A395" s="1" t="s">
         <v>408</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D395" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E395" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
         <v>409</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D396" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A397" s="1" t="s">
         <v>410</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D397" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E397" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
         <v>411</v>
       </c>
       <c r="C398" s="2" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D398" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E398" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F398" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A399" s="1" t="s">
         <v>412</v>
       </c>
       <c r="C399" s="2" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D399" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E399" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F399" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A400" s="1" t="s">
         <v>413</v>
       </c>
       <c r="C400" s="2" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D400" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E400" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A401" s="1" t="s">
         <v>414</v>
       </c>
       <c r="C401" s="2" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D401" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A402" s="1" t="s">
         <v>415</v>
       </c>
       <c r="C402" s="2" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D402" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E402" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F402" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A403" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C403" s="2" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D403" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A404" s="1" t="s">
         <v>416</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D404" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E404" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A405" s="1" t="s">
         <v>417</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D405" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E405" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
         <v>418</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>833</v>
       </c>
-    </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D406" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E406" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A407" s="1" t="s">
         <v>419</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>834</v>
       </c>
-    </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D407" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E407" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
         <v>420</v>
       </c>
       <c r="C408" s="2" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D408" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
         <v>421</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D409" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E409" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>837</v>
       </c>
-    </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D410" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A411" s="1" t="s">
         <v>423</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D411" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
         <v>424</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>839</v>
       </c>
-    </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D412" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E412" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A413" s="1" t="s">
         <v>425</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>840</v>
       </c>
-    </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D413" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E413" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F413" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A414" s="1" t="s">
         <v>426</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>841</v>
       </c>
-    </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D414" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A415" s="1" t="s">
         <v>427</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>842</v>
       </c>
-    </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D415" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A416" s="1" t="s">
         <v>428</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>843</v>
       </c>
-    </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D416" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A417" s="1" t="s">
         <v>429</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D417" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A418" s="1" t="s">
         <v>430</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>844</v>
+      </c>
+      <c r="D418" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -7738,7 +8316,7 @@
           <x14:formula1>
             <xm:f>'Vocabulary Metadata'!$G$2:$G$9</xm:f>
           </x14:formula1>
-          <xm:sqref>D2466:H6138 D2:H2465</xm:sqref>
+          <xm:sqref>D2:H6138</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>